<commit_message>
se agregan validaciones numericas al  formulario de ventas
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\comer\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E24A76-81EA-4869-B270-126869986BD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{8F642101-E425-41E4-B2BC-052E2EB38E17}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -72,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -82,12 +81,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -102,8 +107,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,79 +428,80 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CE445F-108E-4BA1-B118-A498737EB6C3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="150.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega la pregunta de si quiere facturar la venta al realizar una venta
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -432,7 +432,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +471,7 @@
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se desarrollan 2 cancelar factura y el modulo de administracion de clientes
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\comer\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF971DE-A238-4977-9713-0006309F7DCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -81,7 +82,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -91,6 +92,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -107,12 +114,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -428,11 +438,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +456,7 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -496,7 +506,7 @@
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se corrije lo de la facturacion
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF971DE-A238-4977-9713-0006309F7DCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BA35A8-737A-43B4-B02B-19385FB69D75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Acutalizar icono de agregar en todos los apartados , cambiar por un singno de mas  o la palabrea a agregar o el icono de mas la palabra</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Modulo Descuentos a clientes ,en este aparatdo se darian de alta los tipos de clientes con sus respecitvos descuentos que mas adelante cuando  des de alta un cliente en el apartado tipo cliente deberia de salir los de esta tabla</t>
   </si>
   <si>
-    <t>Modulo de Estaciones: aquí  falta un combo  con la sucursal, ya vi que tienes el de alamacen, en este caso  en el combo de alamcen debes de mostrar todos los que sean igual al tipo de almacen " tienda" y mostrar el de la sucursal desabilitado el de alamcen no por si tiene 3 tiendas eleijan  cual</t>
-  </si>
-  <si>
     <t>Modulo de Ventas: el de la cantidad me permite escribir letras</t>
   </si>
   <si>
@@ -67,6 +64,42 @@
   </si>
   <si>
     <t>cancelar facturacion</t>
+  </si>
+  <si>
+    <t>Agregar Bitcoras</t>
+  </si>
+  <si>
+    <t>Modulo de Ventas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calcular un rango en automatico del mayor hacia el infinito </t>
+  </si>
+  <si>
+    <t>Modulo de Usuarios</t>
+  </si>
+  <si>
+    <t>Cambiar al secuencia de los combos 1.- Alamcen , Sucursal  , Rol y hacerlos dependientes uno de cada uno es decir primero seleccionar Sucursal , Luego Almacen , y por ultimo el rol , no puede seleccionar ninguno otra opcion si no esta seleccionada una sucursal, tambien agregar un item que diga --Selecciona--</t>
+  </si>
+  <si>
+    <t>Cuando agrego un usuario con el rol de montacargista la tabla lo pinta como sin rol</t>
+  </si>
+  <si>
+    <t>Modulo Agregar Estacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debe aparece el combo de sucursucal seleccionada la sucursal 1 o la predeterminda de solo lectura </t>
+  </si>
+  <si>
+    <t>Modulo Descuentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agregar la funcion de Agregar o descativar el Descuento </t>
+  </si>
+  <si>
+    <t>Todos los Modulos</t>
+  </si>
+  <si>
+    <t>Los input type que son de numeros solo aceptar numeros con 2 decimales</t>
   </si>
 </sst>
 </file>
@@ -439,75 +472,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A14" sqref="A14:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="150.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="138.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agregan actividades al modulo de ventas
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BA35A8-737A-43B4-B02B-19385FB69D75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2ADC8F-153E-4F35-BCC0-60175DFA0149}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Modulo de Ventas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,16 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
-  <si>
-    <t>Acutalizar icono de agregar en todos los apartados , cambiar por un singno de mas  o la palabrea a agregar o el icono de mas la palabra</t>
-  </si>
-  <si>
-    <t>Modulo Descuentos a clientes ,en este aparatdo se darian de alta los tipos de clientes con sus respecitvos descuentos que mas adelante cuando  des de alta un cliente en el apartado tipo cliente deberia de salir los de esta tabla</t>
-  </si>
-  <si>
-    <t>Modulo de Ventas: el de la cantidad me permite escribir letras</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>Modulo Ventas: Agrega Campo para introducir cuanto le estan pagando y el sistema le diga cuando le corresponde de cambios</t>
   </si>
@@ -57,9 +49,6 @@
     <t xml:space="preserve">Desarrollo los querys del dashboard (1.-Cuanto llevan vendido las estaciones por diaen tiempo real, 2.-Top 5 de los productos vendidos  tiempo real , Top 5 de Clientes mensuales, Venta Total en tiempo real) en tiempo real me refiero que la query es al dia de hoy </t>
   </si>
   <si>
-    <t xml:space="preserve">Modulo Ventas:Cuando se realiza la venta preguntar si quiere facturar </t>
-  </si>
-  <si>
     <t>Agregar loader en todas las peticiones por ajax</t>
   </si>
   <si>
@@ -100,6 +89,99 @@
   </si>
   <si>
     <t>Los input type que son de numeros solo aceptar numeros con 2 decimales</t>
+  </si>
+  <si>
+    <t>Modulo de dashboard</t>
+  </si>
+  <si>
+    <t>Todo el sistema</t>
+  </si>
+  <si>
+    <t>Modulo de ventas</t>
+  </si>
+  <si>
+    <t>agregar Async en todas las peticiones</t>
+  </si>
+  <si>
+    <t>Menudeo</t>
+  </si>
+  <si>
+    <t>Metrica</t>
+  </si>
+  <si>
+    <t>TotalPiezas &gt;=12</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>1 a 11</t>
+  </si>
+  <si>
+    <t>Costo / trapero</t>
+  </si>
+  <si>
+    <t>Rangos</t>
+  </si>
+  <si>
+    <t>Costo/Escoba</t>
+  </si>
+  <si>
+    <t>Venta</t>
+  </si>
+  <si>
+    <t>Cantidad Producto</t>
+  </si>
+  <si>
+    <t>Traperos</t>
+  </si>
+  <si>
+    <t>Escobas</t>
+  </si>
+  <si>
+    <t>cuchara</t>
+  </si>
+  <si>
+    <t>costo/cuchara</t>
+  </si>
+  <si>
+    <t>costo/cubeta</t>
+  </si>
+  <si>
+    <t>cubetas</t>
+  </si>
+  <si>
+    <t>Se debene ajustar los rangos de precios  debido a que existe un rango individual por productos, y una rango por cantidad de productos comprados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agregar combo de uso de cfdi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">agregar un check de desea factura  y quitar la venta de pregunta </t>
+  </si>
+  <si>
+    <t>Si desea factura debemos agregar el iva al producto si no factura no se carga el iva al  producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agrear modal en editar ventas para la factura parar agregar el uso del cfdi, costo del iva </t>
+  </si>
+  <si>
+    <t>Agregar funcionalidad para cobro de iva en ventas , pasadas al dia de hoy , agregar un modal para uso de cfdi , generar el iva, la cajera lo recibe mostrar un input para dar cambio</t>
+  </si>
+  <si>
+    <t>Agregar funcionalidad para buscar productos , en sus diferentes ubicaciones , y sus diferentes costos</t>
+  </si>
+  <si>
+    <t>Cierre de caja  por exceso de efectivo ellos retiran dinero -&gt; guardado en la base de datos por dia hay de cuanto hizo el cierre , puede aver n por dia</t>
+  </si>
+  <si>
+    <t>Cierra de caja  al final del dia  -&gt; cuanto dinero tiene actualmente mas la sumatoria de los cierra por exceso de efectivo+</t>
+  </si>
+  <si>
+    <t>Productos en el ticket visualizar el ahorro del producto cuando existe descuento  por producto al final hacer la cuenta de el total menos el descuento igual a lo que tiene que pagar</t>
+  </si>
+  <si>
+    <t>Menu de control de television, para buscar producto con sus detalles y los cierres de caja</t>
   </si>
 </sst>
 </file>
@@ -115,18 +197,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -147,16 +223,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,127 +545,401 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="138.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
+      <c r="B13" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A14" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5D3FDA7-F80E-4CF3-BEA5-B6A446AE2A18}">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2">
+        <v>3.5</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>14</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3">
+        <f>H3*C2</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4">
+        <f>D2*H4</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>25</v>
+      </c>
+      <c r="C5">
+        <v>2.5</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5">
+        <f>H5*E3</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6">
+        <f>F6*H6</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B9:H14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
se agregan los badges para los roles en la vista de usuarios, se modifica el excel de actividades
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\comer\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2ADC8F-153E-4F35-BCC0-60175DFA0149}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Modulo de Ventas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Modulo Ventas: Agrega Campo para introducir cuanto le estan pagando y el sistema le diga cuando le corresponde de cambios</t>
   </si>
@@ -55,12 +54,6 @@
     <t>cancelar facturacion</t>
   </si>
   <si>
-    <t>Agregar Bitcoras</t>
-  </si>
-  <si>
-    <t>Modulo de Ventas</t>
-  </si>
-  <si>
     <t xml:space="preserve">Calcular un rango en automatico del mayor hacia el infinito </t>
   </si>
   <si>
@@ -70,9 +63,6 @@
     <t>Cambiar al secuencia de los combos 1.- Alamcen , Sucursal  , Rol y hacerlos dependientes uno de cada uno es decir primero seleccionar Sucursal , Luego Almacen , y por ultimo el rol , no puede seleccionar ninguno otra opcion si no esta seleccionada una sucursal, tambien agregar un item que diga --Selecciona--</t>
   </si>
   <si>
-    <t>Cuando agrego un usuario con el rol de montacargista la tabla lo pinta como sin rol</t>
-  </si>
-  <si>
     <t>Modulo Agregar Estacion</t>
   </si>
   <si>
@@ -97,9 +87,6 @@
     <t>Todo el sistema</t>
   </si>
   <si>
-    <t>Modulo de ventas</t>
-  </si>
-  <si>
     <t>agregar Async en todas las peticiones</t>
   </si>
   <si>
@@ -182,12 +169,18 @@
   </si>
   <si>
     <t>Menu de control de television, para buscar producto con sus detalles y los cierres de caja</t>
+  </si>
+  <si>
+    <t>Agregar Modulo Bitcoras</t>
+  </si>
+  <si>
+    <t>Agregar PDF impresión de codigos de barras al modulo de productos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -544,11 +537,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,76 +556,67 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
@@ -640,23 +624,10 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -666,11 +637,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5D3FDA7-F80E-4CF3-BEA5-B6A446AE2A18}">
-  <dimension ref="A1:J26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,30 +655,30 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C2">
         <v>3.5</v>
@@ -722,15 +693,15 @@
         <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -748,7 +719,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J3">
         <f>H3*C2</f>
@@ -757,13 +728,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J4">
         <f>D2*H4</f>
@@ -793,7 +764,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="J5">
         <f>H5*E3</f>
@@ -823,7 +794,7 @@
         <v>9</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J6">
         <f>F6*H6</f>
@@ -832,7 +803,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -888,52 +859,72 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se suben modificaciones en el excel
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\comer\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aoaj720209\Documents\proyectos\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>Modulo Ventas: Agrega Campo para introducir cuanto le estan pagando y el sistema le diga cuando le corresponde de cambios</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>Agregar PDF impresión de codigos de barras al modulo de productos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agregar </t>
+  </si>
+  <si>
+    <t>Agregar compras , idproveddor , producto cantidad precion productos fecha alta, estatus de compra  filtro proveedor rango de fechas y producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ver facturas , estatus facturada cancelada o con error  rango de fechas </t>
   </si>
 </sst>
 </file>
@@ -540,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,15 +567,24 @@
       <c r="A2" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -640,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
se agrega actividad de codigo de barras
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>Modulo Ventas: Agrega Campo para introducir cuanto le estan pagando y el sistema le diga cuando le corresponde de cambios</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>Agregar PDF impresión de codigos de barras al modulo de productos</t>
+  </si>
+  <si>
+    <t>agregar log para cuando se da de alta un producto( cuando aumenta el inventario)</t>
   </si>
 </sst>
 </file>
@@ -638,7 +641,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
@@ -927,6 +930,11 @@
         <v>47</v>
       </c>
     </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B9:H14"/>

</xml_diff>

<commit_message>
se agrega uso de cfdi, se inicia con la reestructura de precios de productos
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\comer\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3C0180-65D9-441B-8050-119D8E03491D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DB4B21-0426-4AEC-B69C-1EE29AEA1833}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Modulo de Ventas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -197,7 +199,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,6 +209,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -223,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -231,6 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,7 +556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -650,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:A31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,12 +877,12 @@
       <c r="H14" s="4"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se ajusta vista de rangos de precios por reestructura
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aoaj720209\Documents\proyectos\comercializadora\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\comer\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E0EB6F-249D-4E81-8B53-5CDA5B714903}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Modulo de Ventas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -191,7 +192,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -233,14 +234,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,10 +561,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -661,11 +667,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,6 +681,7 @@
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -826,139 +833,304 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>48</v>
       </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="16">
+    <mergeCell ref="A31:K31"/>
+    <mergeCell ref="A26:K26"/>
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="A28:K28"/>
+    <mergeCell ref="A29:K29"/>
+    <mergeCell ref="A30:K30"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A25:K25"/>
     <mergeCell ref="B9:H14"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="A19:K19"/>
+    <mergeCell ref="A20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se modifica archivo de avance
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\comer\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yessy\Desktop\PROYECTO\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E0EB6F-249D-4E81-8B53-5CDA5B714903}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C76E2A6-C179-412E-8533-CF55C15C108F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Modulo de Ventas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>Modulo Ventas: Agrega Campo para introducir cuanto le estan pagando y el sistema le diga cuando le corresponde de cambios</t>
   </si>
@@ -186,7 +184,10 @@
     <t>agregar el combo de la sucursal para que pueda seleccionar el alamcen tipo tienda que le corresponde</t>
   </si>
   <si>
-    <t>90% Falta permitir hacer busquedad sin fechas,validar sesion activa</t>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Inicio</t>
   </si>
 </sst>
 </file>
@@ -202,7 +203,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,6 +222,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -234,20 +241,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,16 +593,19 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -670,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:K17"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,304 +845,304 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B9:H14"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="A19:K19"/>
+    <mergeCell ref="A20:K20"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A25:K25"/>
     <mergeCell ref="A31:K31"/>
     <mergeCell ref="A26:K26"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="A29:K29"/>
     <mergeCell ref="A30:K30"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="B9:H14"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A19:K19"/>
-    <mergeCell ref="A20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se actualizan estatus en el archivo de actividades
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\comer\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yessy\Desktop\PROYECTO\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256298EE-0843-4777-B72E-39476B6D01E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD520D18-0B4C-4AE1-A3A8-6274BD1CC93C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Modulo de Ventas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Modulo Ventas: Agrega Campo para introducir cuanto le estan pagando y el sistema le diga cuando le corresponde de cambios</t>
   </si>
@@ -174,9 +172,6 @@
     <t>Menu de control de television, para buscar producto con sus detalles y los cierres de caja</t>
   </si>
   <si>
-    <t>Agregar Modulo Bitcoras</t>
-  </si>
-  <si>
     <t>Agregar PDF impresión de codigos de barras al modulo de productos</t>
   </si>
   <si>
@@ -189,10 +184,13 @@
     <t>OK</t>
   </si>
   <si>
-    <t>Inicio</t>
-  </si>
-  <si>
     <t>falta bd</t>
+  </si>
+  <si>
+    <t>En curso</t>
+  </si>
+  <si>
+    <t>Agregar Modulo Bitacoras</t>
   </si>
 </sst>
 </file>
@@ -253,10 +251,10 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -578,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +592,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -602,15 +603,15 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>51</v>
+      <c r="B4" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -642,7 +643,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -687,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:K28"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,254 +907,254 @@
       <c r="H14" s="8"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
       <c r="L19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
       <c r="L25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B9:H14"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="A19:K19"/>
+    <mergeCell ref="A20:K20"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A25:K25"/>
     <mergeCell ref="A31:K31"/>
     <mergeCell ref="A26:K26"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="A29:K29"/>
     <mergeCell ref="A30:K30"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="B9:H14"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A19:K19"/>
-    <mergeCell ref="A20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se actualizan actividades y se definen cuales seran para el 20 de mayo
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yessy\Desktop\PROYECTO\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD520D18-0B4C-4AE1-A3A8-6274BD1CC93C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1079BA-D163-49D3-9683-071D024DBB32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
   <si>
     <t>Modulo Ventas: Agrega Campo para introducir cuanto le estan pagando y el sistema le diga cuando le corresponde de cambios</t>
   </si>
@@ -187,10 +187,13 @@
     <t>falta bd</t>
   </si>
   <si>
-    <t>En curso</t>
-  </si>
-  <si>
     <t>Agregar Modulo Bitacoras</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>para el 20 de mayo</t>
   </si>
 </sst>
 </file>
@@ -206,7 +209,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,6 +234,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -244,22 +253,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,31 +584,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.140625" style="2" customWidth="1"/>
+    <col min="1" max="2" width="37.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -606,7 +619,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -614,67 +627,79 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -851,60 +876,60 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
@@ -955,79 +980,79 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
@@ -1048,19 +1073,19 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
@@ -1093,68 +1118,68 @@
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B9:H14"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A19:K19"/>
-    <mergeCell ref="A20:K20"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A25:K25"/>
     <mergeCell ref="A31:K31"/>
     <mergeCell ref="A26:K26"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="A29:K29"/>
     <mergeCell ref="A30:K30"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="B9:H14"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="A19:K19"/>
+    <mergeCell ref="A20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se agregan los servcios para la bitacora en la app
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yessy\Desktop\PROYECTO\comercializadora\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1079BA-D163-49D3-9683-071D024DBB32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FCC89A-E7DB-46AC-9696-5ECAEEABEDD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
   <si>
     <t>Modulo Ventas: Agrega Campo para introducir cuanto le estan pagando y el sistema le diga cuando le corresponde de cambios</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>para el 20 de mayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faltan ver la cantidad de productos en alamcenes </t>
   </si>
 </sst>
 </file>
@@ -260,6 +263,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -269,7 +273,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,15 +587,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="37.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="46.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -631,7 +635,7 @@
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="6" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -642,7 +646,7 @@
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>53</v>
       </c>
       <c r="C6" t="s">
@@ -653,7 +657,7 @@
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="6" t="s">
         <v>53</v>
       </c>
       <c r="C7" t="s">
@@ -664,7 +668,7 @@
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>53</v>
       </c>
       <c r="C8" t="s">
@@ -701,6 +705,11 @@
       </c>
       <c r="C12" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -713,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:K19"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,291 +885,291 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
       <c r="L19" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
       <c r="L25" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="16">

</xml_diff>

<commit_message>
Se continua con el modal de consulta de existencias en el modulo de ventas, (falta pintar el rango de precios)
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\comer\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FCC89A-E7DB-46AC-9696-5ECAEEABEDD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9C70B8-D8C2-46D7-9EB0-F95A0E86748C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Modulo de Ventas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -264,14 +266,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -589,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:K20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,60 +887,60 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
@@ -989,79 +991,79 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
@@ -1082,19 +1084,19 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
@@ -1127,68 +1129,68 @@
       <c r="K28" s="8"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B9:H14"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="A19:K19"/>
+    <mergeCell ref="A20:K20"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A25:K25"/>
     <mergeCell ref="A31:K31"/>
     <mergeCell ref="A26:K26"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="A29:K29"/>
     <mergeCell ref="A30:K30"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="B9:H14"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A19:K19"/>
-    <mergeCell ref="A20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se actualiza el excel de actividades
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\comer\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yessy\Desktop\PROYECTO\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9C70B8-D8C2-46D7-9EB0-F95A0E86748C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE2437A-7EEC-49DE-899E-FE138583254E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Modulo de Ventas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>Modulo Ventas: Agrega Campo para introducir cuanto le estan pagando y el sistema le diga cuando le corresponde de cambios</t>
   </si>
@@ -199,6 +197,9 @@
   </si>
   <si>
     <t xml:space="preserve">Faltan ver la cantidad de productos en alamcenes </t>
+  </si>
+  <si>
+    <t>Cambia icon de no resultados</t>
   </si>
 </sst>
 </file>
@@ -589,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,11 +635,11 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>53</v>
+      <c r="B5" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>4</v>
@@ -712,6 +713,14 @@
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -724,7 +733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A22" sqref="A22:K22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
se inicia funcionalidad de retiro de efectivo, faltan detalles
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yessy\Desktop\PROYECTO\comercializadora\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\comer\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85AC80B8-9726-46ED-B329-2E8286DB9D9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0BA09E-70C2-4773-BEDD-267B8F041F2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Modulo de Ventas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
   <si>
     <t>Modulo Ventas: Agrega Campo para introducir cuanto le estan pagando y el sistema le diga cuando le corresponde de cambios</t>
   </si>
@@ -182,9 +184,6 @@
   </si>
   <si>
     <t>OK</t>
-  </si>
-  <si>
-    <t>falta bd</t>
   </si>
   <si>
     <t>Agregar Modulo Bitacoras</t>
@@ -269,14 +268,14 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -594,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,12 +608,12 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>49</v>
@@ -708,7 +707,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>49</v>
@@ -719,23 +718,23 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
         <v>55</v>
-      </c>
-      <c r="C15" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
         <v>57</v>
-      </c>
-      <c r="C16" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -746,10 +745,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:K22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19:L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,62 +910,62 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>36</v>
       </c>
@@ -981,7 +980,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>37</v>
       </c>
@@ -996,7 +995,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>38</v>
       </c>
@@ -1010,11 +1009,8 @@
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
-      <c r="L19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>39</v>
       </c>
@@ -1029,7 +1025,7 @@
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>40</v>
       </c>
@@ -1044,52 +1040,52 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>44</v>
       </c>
@@ -1103,26 +1099,23 @@
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
-      <c r="L25" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>7</v>
       </c>
@@ -1137,7 +1130,7 @@
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>0</v>
       </c>
@@ -1152,69 +1145,69 @@
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B9:H14"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A19:K19"/>
-    <mergeCell ref="A20:K20"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A25:K25"/>
     <mergeCell ref="A31:K31"/>
     <mergeCell ref="A26:K26"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="A29:K29"/>
     <mergeCell ref="A30:K30"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="B9:H14"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="A19:K19"/>
+    <mergeCell ref="A20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se afinin detalles para el retiro por exceso de efectivo
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\comer\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\comer\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0BA09E-70C2-4773-BEDD-267B8F041F2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Modulo de Ventas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
   <si>
     <t>Modulo Ventas: Agrega Campo para introducir cuanto le estan pagando y el sistema le diga cuando le corresponde de cambios</t>
   </si>
@@ -208,12 +207,18 @@
   </si>
   <si>
     <t>Combo de productos agregar ajax para que permita buscar por descripcion ya que solo carga 50</t>
+  </si>
+  <si>
+    <t>falta mostrar los rangos de precios</t>
+  </si>
+  <si>
+    <t>&lt;&lt;-- este no era en otro modulo?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -268,14 +273,14 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,7 +595,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -744,11 +749,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19:L26"/>
+      <selection activeCell="A24" sqref="A24:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,62 +915,62 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>36</v>
       </c>
@@ -980,7 +985,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>37</v>
       </c>
@@ -995,7 +1000,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>38</v>
       </c>
@@ -1010,7 +1015,7 @@
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>39</v>
       </c>
@@ -1025,7 +1030,7 @@
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>40</v>
       </c>
@@ -1040,52 +1045,55 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>44</v>
       </c>
@@ -1100,22 +1108,22 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>7</v>
       </c>
@@ -1130,7 +1138,7 @@
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>0</v>
       </c>
@@ -1145,22 +1153,22 @@
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>46</v>
       </c>
@@ -1175,39 +1183,42 @@
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B9:H14"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="A19:K19"/>
+    <mergeCell ref="A20:K20"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A25:K25"/>
     <mergeCell ref="A31:K31"/>
     <mergeCell ref="A26:K26"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="A29:K29"/>
     <mergeCell ref="A30:K30"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="B9:H14"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A19:K19"/>
-    <mergeCell ref="A20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se termina el cierre de dia y el rango de precios en consulta de existencias en el modulo de ventas
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>Modulo Ventas: Agrega Campo para introducir cuanto le estan pagando y el sistema le diga cuando le corresponde de cambios</t>
   </si>
@@ -207,9 +207,6 @@
   </si>
   <si>
     <t>Combo de productos agregar ajax para que permita buscar por descripcion ya que solo carga 50</t>
-  </si>
-  <si>
-    <t>falta mostrar los rangos de precios</t>
   </si>
   <si>
     <t>&lt;&lt;-- este no era en otro modulo?</t>
@@ -273,14 +270,14 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -753,7 +750,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:K24"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,60 +912,60 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
@@ -1059,9 +1056,6 @@
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
-      <c r="L22" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
@@ -1079,19 +1073,19 @@
       <c r="K23" s="7"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
@@ -1154,19 +1148,19 @@
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
@@ -1184,41 +1178,41 @@
       <c r="K30" s="7"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
       <c r="L31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B9:H14"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A19:K19"/>
-    <mergeCell ref="A20:K20"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A25:K25"/>
     <mergeCell ref="A31:K31"/>
     <mergeCell ref="A26:K26"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="A29:K29"/>
     <mergeCell ref="A30:K30"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="B9:H14"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="A19:K19"/>
+    <mergeCell ref="A20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agrega ordena formulario en el modulo de usuarios dejando por default la sucursal 1, se corrigen detalles
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\comer\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yessy\Desktop\PROYECTO\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D195E51-5C35-4934-B8AF-2D1334E01787}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Modulo de Ventas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
   <si>
     <t>Modulo Ventas: Agrega Campo para introducir cuanto le estan pagando y el sistema le diga cuando le corresponde de cambios</t>
   </si>
@@ -215,7 +214,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -270,14 +269,14 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -592,17 +591,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="37.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -649,16 +649,22 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>8</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -716,16 +722,22 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="4" t="s">
         <v>17</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="C14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="4" t="s">
         <v>54</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="C15" t="s">
         <v>55</v>
@@ -746,10 +758,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
@@ -912,60 +924,60 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
@@ -1148,19 +1160,19 @@
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
@@ -1178,41 +1190,41 @@
       <c r="K30" s="7"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
       <c r="L31" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B9:H14"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="A19:K19"/>
+    <mergeCell ref="A20:K20"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A25:K25"/>
     <mergeCell ref="A31:K31"/>
     <mergeCell ref="A26:K26"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="A29:K29"/>
     <mergeCell ref="A30:K30"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="B9:H14"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A19:K19"/>
-    <mergeCell ref="A20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se modifican inputs para que solo se permita capturar numeros
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yessy\Desktop\PROYECTO\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D195E51-5C35-4934-B8AF-2D1334E01787}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186102FE-0108-4F87-8572-7761113DEAFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
   <si>
     <t>Modulo Ventas: Agrega Campo para introducir cuanto le estan pagando y el sistema le diga cuando le corresponde de cambios</t>
   </si>
@@ -269,14 +269,14 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -595,7 +595,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,8 +690,11 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>17</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -924,60 +927,60 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
@@ -1160,19 +1163,19 @@
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
@@ -1190,41 +1193,41 @@
       <c r="K30" s="7"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
       <c r="L31" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B9:H14"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A19:K19"/>
-    <mergeCell ref="A20:K20"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A25:K25"/>
     <mergeCell ref="A31:K31"/>
     <mergeCell ref="A26:K26"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="A29:K29"/>
     <mergeCell ref="A30:K30"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="B9:H14"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="A19:K19"/>
+    <mergeCell ref="A20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se actualiza excel de actividades
</commit_message>
<xml_diff>
--- a/Analisis/Actividades3.xlsx
+++ b/Analisis/Actividades3.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yessy\Desktop\PROYECTO\comercializadora\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\comer\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186102FE-0108-4F87-8572-7761113DEAFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CF9877-E9CE-43BD-9F08-930221433793}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Modulo de Ventas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -269,14 +271,14 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -594,7 +596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -764,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,60 +929,60 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
@@ -1163,19 +1165,19 @@
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
@@ -1193,41 +1195,41 @@
       <c r="K30" s="7"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
       <c r="L31" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B9:H14"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="A19:K19"/>
+    <mergeCell ref="A20:K20"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A25:K25"/>
     <mergeCell ref="A31:K31"/>
     <mergeCell ref="A26:K26"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="A29:K29"/>
     <mergeCell ref="A30:K30"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="B9:H14"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A19:K19"/>
-    <mergeCell ref="A20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>